<commit_message>
Add < and > to the font
</commit_message>
<xml_diff>
--- a/Font4x6.xlsx
+++ b/Font4x6.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonholmes/Documents/GitHub/Font4x6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\arduino\Arduboy\Font4x6\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6D29F7-4125-42C2-AD59-A39CF83CC0E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="460" windowWidth="38040" windowHeight="25980"/>
+    <workbookView xWindow="9180" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="10" r:id="rId1"/>
@@ -23,13 +24,19 @@
     <definedName name="LS_LR_MIN">#REF!</definedName>
     <definedName name="lSMIN">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -39,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="1">
   <si>
     <t>¢</t>
   </si>
@@ -47,8 +54,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1056,16 +1063,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V48" sqref="V48"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="BE26" sqref="BE26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:106">
+    <row r="1" spans="1:106" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2">
@@ -1202,7 +1209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:106" ht="16">
+    <row r="2" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1420,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:106" ht="16">
+    <row r="3" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1593,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:106" ht="16">
+    <row r="4" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1775,7 +1782,7 @@
       </c>
       <c r="DA4" s="6"/>
     </row>
-    <row r="5" spans="1:106" ht="16">
+    <row r="5" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -1946,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:106" ht="16">
+    <row r="6" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>16</v>
       </c>
@@ -2114,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:106" ht="16">
+    <row r="7" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>32</v>
       </c>
@@ -2312,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:106" ht="16">
+    <row r="8" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>64</v>
       </c>
@@ -2363,7 +2370,7 @@
       <c r="AT8" s="6"/>
       <c r="AU8" s="6"/>
     </row>
-    <row r="9" spans="1:106" ht="16">
+    <row r="9" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>128</v>
       </c>
@@ -2414,7 +2421,7 @@
       <c r="AT9" s="6"/>
       <c r="AU9" s="6"/>
     </row>
-    <row r="10" spans="1:106">
+    <row r="10" spans="1:106" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="str">
@@ -2834,7 +2841,7 @@
         <v>0x21,</v>
       </c>
     </row>
-    <row r="12" spans="1:106">
+    <row r="12" spans="1:106" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2">
@@ -2971,7 +2978,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:106" ht="16">
+    <row r="13" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -3080,7 +3087,7 @@
       <c r="DA13" s="6"/>
       <c r="DB13" s="6"/>
     </row>
-    <row r="14" spans="1:106" ht="16">
+    <row r="14" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -3276,7 +3283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:106" ht="16">
+    <row r="15" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -3474,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:106" ht="16">
+    <row r="16" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -3654,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:106" ht="16">
+    <row r="17" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3830,7 +3837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:106" ht="16">
+    <row r="18" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>32</v>
       </c>
@@ -4031,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:106" ht="16">
+    <row r="19" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>64</v>
       </c>
@@ -4111,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:106" ht="16">
+    <row r="20" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>128</v>
       </c>
@@ -4162,7 +4169,7 @@
       <c r="AT20" s="6"/>
       <c r="AU20" s="6"/>
     </row>
-    <row r="21" spans="1:106">
+    <row r="21" spans="1:106" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="str">
@@ -4582,7 +4589,7 @@
         <v>0x22,</v>
       </c>
     </row>
-    <row r="23" spans="1:106">
+    <row r="23" spans="1:106" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2">
@@ -4690,7 +4697,9 @@
       <c r="AK23" s="2">
         <v>43</v>
       </c>
-      <c r="AL23" s="2"/>
+      <c r="AL23" s="2">
+        <v>44</v>
+      </c>
       <c r="AM23" s="2">
         <v>45</v>
       </c>
@@ -4718,8 +4727,11 @@
       <c r="AU23" s="2">
         <v>55</v>
       </c>
+      <c r="AV23" s="2">
+        <v>56</v>
+      </c>
     </row>
-    <row r="24" spans="1:106" ht="16">
+    <row r="24" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -4852,7 +4864,7 @@
       <c r="DA24" s="6"/>
       <c r="DB24" s="6"/>
     </row>
-    <row r="25" spans="1:106" ht="16">
+    <row r="25" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -4940,11 +4952,14 @@
       <c r="AU25" s="6"/>
       <c r="AV25" s="6"/>
       <c r="AY25" s="6"/>
-      <c r="AZ25" s="6"/>
-      <c r="BA25" s="6"/>
+      <c r="BA25" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="BB25" s="6"/>
       <c r="BC25" s="6"/>
-      <c r="BD25" s="6"/>
+      <c r="BD25" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="BE25" s="6"/>
       <c r="BF25" s="6"/>
       <c r="BG25" s="6"/>
@@ -4984,7 +4999,7 @@
       <c r="DA25" s="6"/>
       <c r="DB25" s="6"/>
     </row>
-    <row r="26" spans="1:106" ht="16">
+    <row r="26" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>4</v>
       </c>
@@ -5076,12 +5091,16 @@
       <c r="AU26" s="6"/>
       <c r="AV26" s="6"/>
       <c r="AY26" s="6"/>
-      <c r="AZ26" s="6"/>
+      <c r="AZ26" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="BA26" s="6"/>
       <c r="BB26" s="6"/>
       <c r="BC26" s="6"/>
       <c r="BD26" s="6"/>
-      <c r="BE26" s="6"/>
+      <c r="BE26" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="BF26" s="6"/>
       <c r="BG26" s="6"/>
       <c r="BJ26" s="6"/>
@@ -5112,7 +5131,7 @@
       <c r="CZ26" s="6"/>
       <c r="DA26" s="6"/>
     </row>
-    <row r="27" spans="1:106" ht="16">
+    <row r="27" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>8</v>
       </c>
@@ -5206,8 +5225,13 @@
       <c r="AU27" s="6"/>
       <c r="AV27" s="6"/>
       <c r="AY27" s="6"/>
-      <c r="BB27" s="6"/>
+      <c r="BA27" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="BC27" s="6"/>
+      <c r="BD27" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="BE27" s="6"/>
       <c r="BF27" s="6"/>
       <c r="BG27" s="6"/>
@@ -5240,7 +5264,7 @@
       <c r="CX27" s="6"/>
       <c r="CZ27" s="6"/>
     </row>
-    <row r="28" spans="1:106" ht="16">
+    <row r="28" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>16</v>
       </c>
@@ -5352,7 +5376,7 @@
       <c r="CX28" s="6"/>
       <c r="CY28" s="6"/>
     </row>
-    <row r="29" spans="1:106" ht="16">
+    <row r="29" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>32</v>
       </c>
@@ -5485,7 +5509,7 @@
       <c r="DA29" s="6"/>
       <c r="DB29" s="6"/>
     </row>
-    <row r="30" spans="1:106" ht="16">
+    <row r="30" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>64</v>
       </c>
@@ -5541,7 +5565,7 @@
       <c r="CV30" s="6"/>
       <c r="CW30" s="6"/>
     </row>
-    <row r="31" spans="1:106" ht="16">
+    <row r="31" spans="1:106" ht="15" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>128</v>
       </c>
@@ -5592,7 +5616,7 @@
       <c r="AT31" s="6"/>
       <c r="AU31" s="6"/>
     </row>
-    <row r="32" spans="1:106">
+    <row r="32" spans="1:106" x14ac:dyDescent="0.45">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5" t="str">
@@ -5793,11 +5817,11 @@
       </c>
       <c r="AZ32" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>0x00,</v>
+        <v>0x04,</v>
       </c>
       <c r="BA32" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>0x00,</v>
+        <v>0x0A,</v>
       </c>
       <c r="BB32" s="5" t="str">
         <f t="shared" si="4"/>
@@ -5809,11 +5833,11 @@
       </c>
       <c r="BD32" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>0x00,</v>
+        <v>0x0A,</v>
       </c>
       <c r="BE32" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>0x00,</v>
+        <v>0x04,</v>
       </c>
       <c r="BF32" s="5" t="str">
         <f t="shared" si="4"/>

</xml_diff>